<commit_message>
Added usecases for multithreading.
</commit_message>
<xml_diff>
--- a/ACE_UseCase_Update.xlsx
+++ b/ACE_UseCase_Update.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>UseCase  : JMS (OrderQueue and ExecutedOrderQueue)</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Hi</t>
+  </si>
+  <si>
+    <t>sangeeta sahu</t>
+  </si>
+  <si>
+    <t>Ravi kant sharma</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +484,35 @@
       </c>
       <c r="D4" s="1">
         <f ca="1">+NOW()</f>
-        <v>42710.645992592596</v>
+        <v>42711.684783101853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42711.684027777781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42711.684027777781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>